<commit_message>
Cedulas pendientes por cerrar sesion x5
</commit_message>
<xml_diff>
--- a/cedulas_cerrar_sesion.xlsx
+++ b/cedulas_cerrar_sesion.xlsx
@@ -1,52 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ContratosSuperflex\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995A86DB-44BB-4898-918A-5ADBEFBEEFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -61,24 +57,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -344,410 +400,414 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A2:A80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <col width="24.77734375" customWidth="1" style="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2">
+      <c r="A2" s="3" t="n">
         <v>21229026</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3">
+      <c r="A3" t="n">
         <v>39727147</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4">
+      <c r="A4" t="n">
         <v>17329021</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5">
+      <c r="A5" t="n">
         <v>39728361</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="6">
+      <c r="A6" t="n">
         <v>40334977</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="7">
+      <c r="A7" t="n">
         <v>1125552959</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8">
+      <c r="A8" t="n">
         <v>1023035549</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9">
+      <c r="A9" t="n">
         <v>38290869</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10">
+      <c r="A10" t="n">
         <v>40386471</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11">
+      <c r="A11" t="n">
         <v>1121946821</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="12">
+      <c r="A12" t="n">
         <v>1007816099</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13">
+      <c r="A13" t="n">
         <v>1006797846</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14">
+      <c r="A14" t="n">
         <v>1006774144</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15">
+      <c r="A15" t="n">
         <v>1121872788</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="16">
+      <c r="A16" t="n">
         <v>24100971</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="17">
+      <c r="A17" t="n">
         <v>1029981260</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18">
+      <c r="A18" t="n">
         <v>1121830619</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="19">
+      <c r="A19" t="n">
         <v>1006794572</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="20">
+      <c r="A20" t="n">
         <v>1006824446</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="21">
+      <c r="A21" t="n">
         <v>1096196072</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="22">
+      <c r="A22" t="n">
         <v>1034660761</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="23">
+      <c r="A23" t="n">
         <v>21205258</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="24">
+      <c r="A24" t="n">
         <v>17360686</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="25">
+      <c r="A25" t="n">
         <v>51642333</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+    <row r="26">
+      <c r="A26" t="n">
         <v>3292415</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+    <row r="27">
+      <c r="A27" t="n">
         <v>11373533</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+    <row r="28">
+      <c r="A28" t="n">
         <v>30030456</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+    <row r="29">
+      <c r="A29" t="n">
         <v>70052315</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+    <row r="30">
+      <c r="A30" t="n">
         <v>3282146</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="31">
+      <c r="A31" t="n">
         <v>3045925</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+    <row r="32">
+      <c r="A32" t="n">
         <v>21173140</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+    <row r="33">
+      <c r="A33" t="n">
         <v>21234532</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+    <row r="34">
+      <c r="A34" t="n">
         <v>6671921</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+    <row r="35">
+      <c r="A35" t="n">
         <v>4561950</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+    <row r="36">
+      <c r="A36" t="n">
         <v>19337954</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+    <row r="37">
+      <c r="A37" t="n">
         <v>40434896</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+    <row r="38">
+      <c r="A38" t="n">
         <v>1123860656</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+    <row r="39">
+      <c r="A39" t="n">
         <v>30055352</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
+    <row r="40">
+      <c r="A40" s="2" t="n">
         <v>59671136</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
+    <row r="41">
+      <c r="A41" s="2" t="n">
         <v>21177991</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
+    <row r="42">
+      <c r="A42" s="2" t="n">
         <v>14993451</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
+    <row r="43">
+      <c r="A43" s="2" t="n">
         <v>40361978</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
+    <row r="44">
+      <c r="A44" s="2" t="n">
         <v>7818547</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
+    <row r="45">
+      <c r="A45" s="2" t="n">
         <v>40412991</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2">
+    <row r="46">
+      <c r="A46" s="2" t="n">
         <v>86040029</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
+    <row r="47">
+      <c r="A47" t="n">
         <v>40265797</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+    <row r="48">
+      <c r="A48" t="n">
         <v>37559806</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
+    <row r="49">
+      <c r="A49" t="n">
         <v>79849312</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
+    <row r="50">
+      <c r="A50" t="n">
         <v>1121148787</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
+    <row r="51">
+      <c r="A51" t="n">
         <v>1000807612</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
+    <row r="52">
+      <c r="A52" t="n">
         <v>31006869</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
+    <row r="53">
+      <c r="A53" t="n">
         <v>1124190027</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
+    <row r="54">
+      <c r="A54" t="n">
         <v>40422019</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
+    <row r="55">
+      <c r="A55" t="n">
         <v>1006697169</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
+    <row r="56">
+      <c r="A56" t="n">
         <v>1124216732</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
+    <row r="57">
+      <c r="A57" t="n">
         <v>30081386</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
+    <row r="58">
+      <c r="A58" t="n">
         <v>21940107</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
+    <row r="59">
+      <c r="A59" t="n">
         <v>40433512</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
+    <row r="60">
+      <c r="A60" t="n">
         <v>18598661</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
+    <row r="61">
+      <c r="A61" t="n">
         <v>86009284</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
+    <row r="62">
+      <c r="A62" t="n">
         <v>31006780</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
+    <row r="63">
+      <c r="A63" t="n">
         <v>28845786</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
+    <row r="64">
+      <c r="A64" t="n">
         <v>1120373472</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
+    <row r="65">
+      <c r="A65" t="n">
         <v>14952515</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
+    <row r="66">
+      <c r="A66" t="n">
         <v>1098436557</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
+    <row r="67">
+      <c r="A67" t="n">
         <v>80266280</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
+    <row r="68">
+      <c r="A68" t="n">
         <v>1121875236</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
+    <row r="69">
+      <c r="A69" t="n">
         <v>1123512956</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
+    <row r="70">
+      <c r="A70" t="n">
         <v>1123114061</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
+    <row r="71">
+      <c r="A71" t="n">
         <v>1121903090</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1">
+    <row r="72">
+      <c r="A72" t="n">
         <v>1006697920</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
+    <row r="73">
+      <c r="A73" t="n">
         <v>1123085348</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
+    <row r="74">
+      <c r="A74" t="n">
         <v>1120006623</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1">
+    <row r="75">
+      <c r="A75" t="n">
         <v>1122646404</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
+    <row r="76">
+      <c r="A76" t="n">
         <v>21991161</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
+    <row r="77">
+      <c r="A77" t="n">
         <v>1120381379</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
+    <row r="78">
+      <c r="A78" t="n">
         <v>1121921932</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
+    <row r="79">
+      <c r="A79" t="n">
         <v>1006874253</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
+    <row r="80">
+      <c r="A80" t="n">
         <v>1123567290</v>
       </c>
     </row>

</xml_diff>